<commit_message>
mise à jour de la ligne 2 de clone_dossier'
</commit_message>
<xml_diff>
--- a/fichier.xlsx
+++ b/fichier.xlsx
@@ -16,6 +16,14 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+  <si>
+    <t>Deuxième ligne modifié</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -69,7 +77,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -114,7 +122,7 @@
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="Yu Gothic Light"/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
         <a:font script="Hans" typeface="等线 Light"/>
         <a:font script="Hant" typeface="新細明體"/>
@@ -149,7 +157,7 @@
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="Yu Gothic"/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
         <a:font script="Hans" typeface="等线"/>
         <a:font script="Hant" typeface="新細明體"/>
@@ -331,12 +339,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="26.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
deuxième modification du fichier excel
</commit_message>
<xml_diff>
--- a/fichier.xlsx
+++ b/fichier.xlsx
@@ -19,12 +19,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
   <si>
-    <t>Modification de la ligne 2 dans le dossier devoir</t>
-  </si>
-  <si>
-    <t>conflit résolu</t>
+    <t>Modification de la ligne 2 dans le dossier devoir *2</t>
   </si>
 </sst>
 </file>
@@ -342,10 +339,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:A3"/>
+  <dimension ref="A2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -358,11 +355,6 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>1</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>